<commit_message>
Added ability to add all pdfs into main file
</commit_message>
<xml_diff>
--- a/Submittal Automation/Misc Documents/Key Personnel List.xlsx
+++ b/Submittal Automation/Misc Documents/Key Personnel List.xlsx
@@ -68,10 +68,10 @@
     <t>Yokoi, Ryan K.</t>
   </si>
   <si>
-    <t>Full Title</t>
-  </si>
-  <si>
-    <t>Address</t>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>LONG</t>
   </si>
 </sst>
 </file>
@@ -485,38 +485,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -847,19 +847,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -869,23 +869,23 @@
       <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="A3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="9" t="s">
         <v>1</v>
       </c>
@@ -900,11 +900,11 @@
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
End of the day commit: Finished logfile and insert pages for Submittal Automation
</commit_message>
<xml_diff>
--- a/Submittal Automation/Misc Documents/Key Personnel List.xlsx
+++ b/Submittal Automation/Misc Documents/Key Personnel List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCST-352-BH\Documents\Higashi_Files\Useful\Submittal Automation\Misc Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCST-352-BH\Documents\Higashi_Files\Useful\BCS Programming\Submittal Automation\Misc Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,10 +68,10 @@
     <t>Yokoi, Ryan K.</t>
   </si>
   <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>LONG</t>
+    <t>LONG UH</t>
+  </si>
+  <si>
+    <t>HILO</t>
   </si>
 </sst>
 </file>
@@ -485,38 +485,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -847,19 +847,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -869,23 +869,23 @@
       <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25"/>
+      <c r="A3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="9" t="s">
         <v>1</v>
       </c>
@@ -900,11 +900,11 @@
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Submittal Automation: Made general READability changes, added ToC into main and MISC specref into it
</commit_message>
<xml_diff>
--- a/Submittal Automation/Misc Documents/Key Personnel List.xlsx
+++ b/Submittal Automation/Misc Documents/Key Personnel List.xlsx
@@ -68,10 +68,10 @@
     <t>Yokoi, Ryan K.</t>
   </si>
   <si>
-    <t>LONG UH</t>
-  </si>
-  <si>
-    <t>HILO</t>
+    <t>Full Title</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>

</xml_diff>